<commit_message>
fixes waypoint dist check, _init update and default scene names
</commit_message>
<xml_diff>
--- a/data/nott walking ex.2.xlsx
+++ b/data/nott walking ex.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="39255" yWindow="120" windowWidth="35100" windowHeight="18285" activeTab="2"/>
+    <workbookView xWindow="39255" yWindow="120" windowWidth="35100" windowHeight="18285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="167">
   <si>
     <t>theme</t>
   </si>
@@ -178,9 +178,6 @@
     <t>contextfile</t>
   </si>
   <si>
-    <t>context-test1.json</t>
-  </si>
-  <si>
     <t>startdelay</t>
   </si>
   <si>
@@ -421,9 +418,6 @@
     <t>Theme 1 - strings&amp;piano</t>
   </si>
   <si>
-    <t>NVA</t>
-  </si>
-  <si>
     <t>t4A1.wav</t>
   </si>
   <si>
@@ -527,6 +521,9 @@
   </si>
   <si>
     <t>4d</t>
+  </si>
+  <si>
+    <t>_context-test1.json</t>
   </si>
 </sst>
 </file>
@@ -1666,7 +1663,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,7 +1693,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1704,7 +1701,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1712,7 +1709,7 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1736,7 +1733,7 @@
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1754,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1783,7 +1780,7 @@
         <v>34</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -1825,32 +1822,28 @@
         <v>3</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="5">
-        <v>20</v>
-      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O2" s="8">
         <v>1</v>
@@ -1861,10 +1854,10 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>26</v>
@@ -1876,7 +1869,7 @@
         <v>-1</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O3" s="8">
         <v>1</v>
@@ -1887,25 +1880,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G4" s="3">
         <v>20</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O4" s="8">
         <v>2</v>
@@ -1916,25 +1909,25 @@
     </row>
     <row r="5" spans="1:17" ht="30.75" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G5" s="3">
         <v>10</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O5" s="8">
         <v>3</v>
@@ -1948,7 +1941,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
@@ -1957,13 +1950,13 @@
         <v>26</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G6" s="3">
         <v>20</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>12</v>
@@ -1980,7 +1973,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="3">
         <v>3</v>
@@ -1989,16 +1982,16 @@
         <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G7" s="3">
         <v>20</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O7" s="8">
         <v>1</v>
@@ -2012,22 +2005,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G8" s="3">
         <v>40</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O8" s="8">
         <v>1</v>
@@ -2038,22 +2031,22 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G9" s="3">
         <v>30</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O9" s="8">
         <v>2</v>
@@ -2064,22 +2057,22 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G10" s="3">
         <v>20</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O10" s="8">
         <v>3</v>
@@ -2090,22 +2083,22 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O11" s="8">
         <v>4</v>
@@ -2129,7 +2122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -2192,7 +2185,7 @@
   <sheetData>
     <row r="1" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>10</v>
@@ -2201,16 +2194,16 @@
         <v>22</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>5</v>
@@ -2219,25 +2212,25 @@
         <v>4</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="O1" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="O1" s="14" t="s">
-        <v>114</v>
-      </c>
       <c r="P1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q1" s="14" t="s">
         <v>20</v>
@@ -2246,118 +2239,118 @@
         <v>18</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U1" s="15" t="s">
         <v>17</v>
       </c>
       <c r="V1" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W1" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X1" s="16" t="s">
         <v>18</v>
       </c>
       <c r="Y1" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z1" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AA1" s="17" t="s">
         <v>17</v>
       </c>
       <c r="AB1" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AC1" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AD1" s="18" t="s">
         <v>18</v>
       </c>
       <c r="AE1" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AF1" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AG1" s="19" t="s">
         <v>17</v>
       </c>
       <c r="AH1" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AI1" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AJ1" s="20" t="s">
         <v>18</v>
       </c>
       <c r="AK1" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL1" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AM1" s="21" t="s">
         <v>17</v>
       </c>
       <c r="AN1" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AO1" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AP1" s="22" t="s">
         <v>18</v>
       </c>
       <c r="AQ1" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR1" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AS1" s="23" t="s">
         <v>17</v>
       </c>
       <c r="AT1" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU1" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AV1" s="24" t="s">
         <v>18</v>
       </c>
       <c r="AW1" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AX1" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AY1" s="25" t="s">
         <v>17</v>
       </c>
       <c r="AZ1" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="BA1" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BB1" s="26" t="s">
         <v>18</v>
       </c>
       <c r="BC1" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BD1" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BE1" s="28" t="s">
         <v>17</v>
@@ -2365,10 +2358,10 @@
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="30">
         <v>62</v>
@@ -2377,7 +2370,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" s="31">
         <v>73</v>
@@ -2386,16 +2379,16 @@
         <v>1</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L2" s="33" t="s">
         <v>7</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O2" s="34">
         <v>34</v>
@@ -2406,13 +2399,13 @@
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.3">
       <c r="J3" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K3" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M3" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O3" s="34">
         <v>55</v>
@@ -2432,16 +2425,16 @@
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.3">
       <c r="J4" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L4" s="33" t="s">
         <v>7</v>
       </c>
       <c r="M4" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O4" s="34">
         <v>36.587000000000003</v>
@@ -2458,25 +2451,25 @@
         <v>2</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="31">
         <v>96</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I5" s="32">
         <v>2</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K5" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M5" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N5" s="34">
         <v>96</v>
@@ -2490,25 +2483,25 @@
         <v>3</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="31">
         <v>96</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I6" s="32">
         <v>3</v>
       </c>
       <c r="J6" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K6" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M6" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N6" s="34">
         <v>96</v>
@@ -2519,13 +2512,13 @@
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.3">
       <c r="J7" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K7" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M7" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N7" s="34">
         <v>96</v>
@@ -2539,7 +2532,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="30">
         <v>62</v>
@@ -2548,7 +2541,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="31">
         <v>16</v>
@@ -2560,13 +2553,13 @@
         <v>1</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K8" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M8" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N8" s="34">
         <v>16</v>
@@ -2577,16 +2570,16 @@
     </row>
     <row r="9" spans="1:57" x14ac:dyDescent="0.3">
       <c r="J9" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K9" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L9" s="33" t="s">
         <v>7</v>
       </c>
       <c r="M9" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O9" s="34">
         <v>9</v>
@@ -2597,10 +2590,10 @@
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="30" t="s">
         <v>69</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>70</v>
       </c>
       <c r="C10" s="30">
         <v>62</v>
@@ -2609,7 +2602,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" s="31">
         <v>16</v>
@@ -2621,13 +2614,13 @@
         <v>1</v>
       </c>
       <c r="J10" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K10" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M10" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N10" s="34">
         <v>16</v>
@@ -2638,16 +2631,16 @@
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.3">
       <c r="J11" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K11" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L11" s="33" t="s">
         <v>7</v>
       </c>
       <c r="M11" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O11" s="34">
         <v>10</v>
@@ -2658,10 +2651,10 @@
     </row>
     <row r="12" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="30">
         <v>55</v>
@@ -2670,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F12" s="31">
         <v>54</v>
@@ -2682,13 +2675,13 @@
         <v>1</v>
       </c>
       <c r="J12" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K12" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M12" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N12" s="34">
         <v>54</v>
@@ -2705,19 +2698,19 @@
     </row>
     <row r="13" spans="1:57" x14ac:dyDescent="0.3">
       <c r="E13" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J13" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K13" s="33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L13" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M13" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N13" s="34">
         <v>9</v>
@@ -2726,7 +2719,7 @@
         <v>1</v>
       </c>
       <c r="V13" s="36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="W13" s="36">
         <v>9</v>
@@ -2735,7 +2728,7 @@
         <v>1</v>
       </c>
       <c r="AB13" s="38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AC13" s="38">
         <v>9</v>
@@ -2750,7 +2743,7 @@
         <v>1</v>
       </c>
       <c r="AN13" s="42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AO13" s="42">
         <v>9</v>
@@ -2759,7 +2752,7 @@
         <v>1</v>
       </c>
       <c r="AT13" s="30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AU13" s="30">
         <v>9</v>
@@ -2773,7 +2766,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F14" s="31">
         <v>54</v>
@@ -2785,13 +2778,13 @@
         <v>1</v>
       </c>
       <c r="J14" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M14" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N14" s="34">
         <v>54</v>
@@ -2808,19 +2801,19 @@
     </row>
     <row r="15" spans="1:57" x14ac:dyDescent="0.3">
       <c r="E15" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K15" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L15" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M15" s="34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N15" s="34">
         <v>9</v>
@@ -2829,7 +2822,7 @@
         <v>1</v>
       </c>
       <c r="V15" s="36" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="W15" s="36">
         <v>9</v>
@@ -2838,7 +2831,7 @@
         <v>1</v>
       </c>
       <c r="AB15" s="47" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC15" s="38">
         <v>9</v>
@@ -2853,7 +2846,7 @@
         <v>1</v>
       </c>
       <c r="AN15" s="42" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AO15" s="42">
         <v>9</v>
@@ -2862,7 +2855,7 @@
         <v>1</v>
       </c>
       <c r="AT15" s="30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AU15" s="30">
         <v>9</v>
@@ -2876,7 +2869,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F16" s="31">
         <v>54</v>
@@ -2888,13 +2881,13 @@
         <v>1</v>
       </c>
       <c r="J16" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K16" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M16" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N16" s="34">
         <v>54</v>
@@ -2911,19 +2904,19 @@
     </row>
     <row r="17" spans="4:48" x14ac:dyDescent="0.3">
       <c r="E17" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J17" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K17" s="33" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L17" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M17" s="34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N17" s="34">
         <v>9</v>
@@ -2932,7 +2925,7 @@
         <v>1</v>
       </c>
       <c r="V17" s="36" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="W17" s="36">
         <v>9</v>
@@ -2941,7 +2934,7 @@
         <v>1</v>
       </c>
       <c r="AB17" s="47" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AC17" s="38">
         <v>9</v>
@@ -2956,7 +2949,7 @@
         <v>1</v>
       </c>
       <c r="AN17" s="42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AO17" s="42">
         <v>9</v>
@@ -2965,7 +2958,7 @@
         <v>1</v>
       </c>
       <c r="AT17" s="30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AU17" s="30">
         <v>9</v>
@@ -2979,7 +2972,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F18" s="31">
         <v>54</v>
@@ -2991,13 +2984,13 @@
         <v>1</v>
       </c>
       <c r="J18" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M18" s="34" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N18" s="34">
         <v>54</v>
@@ -3015,16 +3008,16 @@
     </row>
     <row r="19" spans="4:48" x14ac:dyDescent="0.3">
       <c r="E19" s="48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J19" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K19" s="33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="M19" s="34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="N19" s="34">
         <v>54</v>
@@ -3072,16 +3065,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>17</v>
@@ -3131,7 +3124,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3182,7 +3175,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
adds support for endeverybeats; prefers same region at same priority
</commit_message>
<xml_diff>
--- a/data/nott walking ex.2.xlsx
+++ b/data/nott walking ex.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="39255" yWindow="120" windowWidth="35100" windowHeight="18285" activeTab="1"/>
+    <workbookView xWindow="39255" yWindow="120" windowWidth="35100" windowHeight="18285" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="171">
   <si>
     <t>theme</t>
   </si>
@@ -43,9 +43,6 @@
     <t>endbeats</t>
   </si>
   <si>
-    <t>4,8,12,16</t>
-  </si>
-  <si>
     <t>oneshot</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>t3accent1.wav</t>
   </si>
   <si>
-    <t>16,32,48,64,80,96</t>
-  </si>
-  <si>
     <t>t1</t>
   </si>
   <si>
@@ -283,12 +277,6 @@
     <t>pad in Fs</t>
   </si>
   <si>
-    <t>t4padA.wav</t>
-  </si>
-  <si>
-    <t>t4padFs.wav</t>
-  </si>
-  <si>
     <t>1b</t>
   </si>
   <si>
@@ -454,9 +442,6 @@
     <t>t4A6.wav</t>
   </si>
   <si>
-    <t>t4padE.wav</t>
-  </si>
-  <si>
     <t>t4E1.wav</t>
   </si>
   <si>
@@ -524,6 +509,33 @@
   </si>
   <si>
     <t>_context-test1.json</t>
+  </si>
+  <si>
+    <t>t4Apad.wav</t>
+  </si>
+  <si>
+    <t>t4Fspad.wav</t>
+  </si>
+  <si>
+    <t>t4Bpad.wav</t>
+  </si>
+  <si>
+    <t>t4Epad.wav</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test-t1-2</t>
+  </si>
+  <si>
+    <t>test-t1-3</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>endeverybeats</t>
   </si>
 </sst>
 </file>
@@ -1674,66 +1686,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
         <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1749,10 +1761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1777,43 +1789,43 @@
   <sheetData>
     <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>0</v>
@@ -1822,28 +1834,28 @@
         <v>3</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O2" s="8">
         <v>1</v>
@@ -1854,13 +1866,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -1869,7 +1881,7 @@
         <v>-1</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O3" s="8">
         <v>1</v>
@@ -1880,25 +1892,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G4" s="3">
         <v>20</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O4" s="8">
         <v>2</v>
@@ -1909,25 +1921,25 @@
     </row>
     <row r="5" spans="1:17" ht="30.75" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G5" s="3">
         <v>10</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O5" s="8">
         <v>3</v>
@@ -1941,25 +1953,25 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G6" s="3">
         <v>20</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O6" s="8">
         <v>1</v>
@@ -1973,25 +1985,25 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="3">
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G7" s="3">
         <v>20</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O7" s="8">
         <v>1</v>
@@ -2005,22 +2017,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G8" s="3">
         <v>40</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O8" s="8">
         <v>1</v>
@@ -2031,22 +2043,22 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G9" s="3">
         <v>30</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O9" s="8">
         <v>2</v>
@@ -2057,22 +2069,22 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G10" s="3">
         <v>20</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O10" s="8">
         <v>3</v>
@@ -2083,28 +2095,88 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O11" s="8">
         <v>4</v>
       </c>
       <c r="P11" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="O12" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="O13" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2120,10 +2192,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE26"/>
+  <dimension ref="A1:BF26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2135,233 +2207,237 @@
     <col min="5" max="5" width="22.140625" style="31" customWidth="1"/>
     <col min="6" max="6" width="7.140625" style="31" customWidth="1"/>
     <col min="7" max="7" width="10" style="31" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="31" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="32" customWidth="1"/>
-    <col min="10" max="10" width="15" style="33" customWidth="1"/>
-    <col min="11" max="11" width="23" style="33" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="33" customWidth="1"/>
-    <col min="13" max="13" width="17" style="34" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="34" customWidth="1"/>
-    <col min="15" max="15" width="9" style="34" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="34" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="34" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" style="34" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" style="34" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="35" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" style="35" customWidth="1"/>
-    <col min="22" max="22" width="13.42578125" style="36" customWidth="1"/>
-    <col min="23" max="23" width="6.140625" style="36" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" style="36" customWidth="1"/>
-    <col min="25" max="25" width="10.7109375" style="36" customWidth="1"/>
-    <col min="26" max="26" width="13.7109375" style="37" customWidth="1"/>
-    <col min="27" max="27" width="10.42578125" style="37" customWidth="1"/>
-    <col min="28" max="28" width="17" style="38" customWidth="1"/>
-    <col min="29" max="29" width="6.140625" style="38" customWidth="1"/>
-    <col min="30" max="30" width="9.85546875" style="38" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" style="38" customWidth="1"/>
-    <col min="32" max="32" width="13.7109375" style="39" customWidth="1"/>
-    <col min="33" max="33" width="10.42578125" style="39" customWidth="1"/>
-    <col min="34" max="34" width="13.42578125" style="40" customWidth="1"/>
-    <col min="35" max="36" width="8.85546875" style="40"/>
-    <col min="37" max="37" width="10.7109375" style="40" customWidth="1"/>
-    <col min="38" max="38" width="13.7109375" style="41" customWidth="1"/>
-    <col min="39" max="39" width="10.42578125" style="41" customWidth="1"/>
-    <col min="40" max="40" width="14.85546875" style="42" customWidth="1"/>
-    <col min="41" max="42" width="8.85546875" style="42"/>
-    <col min="43" max="43" width="10.7109375" style="42" customWidth="1"/>
-    <col min="44" max="44" width="13.7109375" style="43" customWidth="1"/>
-    <col min="45" max="45" width="10.42578125" style="43" customWidth="1"/>
-    <col min="46" max="46" width="13.140625" style="30" customWidth="1"/>
-    <col min="47" max="48" width="8.85546875" style="30"/>
-    <col min="49" max="49" width="10.7109375" style="30" customWidth="1"/>
-    <col min="50" max="50" width="13.7109375" style="44" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" style="44" customWidth="1"/>
-    <col min="52" max="54" width="8.85546875" style="45"/>
-    <col min="55" max="55" width="10.7109375" style="45" customWidth="1"/>
-    <col min="56" max="56" width="13.7109375" style="46" customWidth="1"/>
-    <col min="57" max="57" width="10.42578125" style="46" customWidth="1"/>
-    <col min="58" max="16384" width="8.85546875" style="3"/>
+    <col min="8" max="8" width="18" style="31" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="31" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="32" customWidth="1"/>
+    <col min="11" max="11" width="15" style="33" customWidth="1"/>
+    <col min="12" max="12" width="23" style="33" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="33" customWidth="1"/>
+    <col min="14" max="14" width="17" style="34" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" style="34" customWidth="1"/>
+    <col min="16" max="16" width="9" style="34" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" style="34" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" style="34" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" style="34" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" style="34" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" style="35" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" style="35" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" style="36" customWidth="1"/>
+    <col min="24" max="24" width="6.140625" style="36" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" style="36" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" style="36" customWidth="1"/>
+    <col min="27" max="27" width="13.7109375" style="37" customWidth="1"/>
+    <col min="28" max="28" width="10.42578125" style="37" customWidth="1"/>
+    <col min="29" max="29" width="17" style="38" customWidth="1"/>
+    <col min="30" max="30" width="6.140625" style="38" customWidth="1"/>
+    <col min="31" max="31" width="9.85546875" style="38" customWidth="1"/>
+    <col min="32" max="32" width="10.7109375" style="38" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" style="39" customWidth="1"/>
+    <col min="34" max="34" width="10.42578125" style="39" customWidth="1"/>
+    <col min="35" max="35" width="13.42578125" style="40" customWidth="1"/>
+    <col min="36" max="37" width="8.85546875" style="40"/>
+    <col min="38" max="38" width="10.7109375" style="40" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" style="41" customWidth="1"/>
+    <col min="40" max="40" width="10.42578125" style="41" customWidth="1"/>
+    <col min="41" max="41" width="14.85546875" style="42" customWidth="1"/>
+    <col min="42" max="43" width="8.85546875" style="42"/>
+    <col min="44" max="44" width="10.7109375" style="42" customWidth="1"/>
+    <col min="45" max="45" width="13.7109375" style="43" customWidth="1"/>
+    <col min="46" max="46" width="10.42578125" style="43" customWidth="1"/>
+    <col min="47" max="47" width="13.140625" style="30" customWidth="1"/>
+    <col min="48" max="49" width="8.85546875" style="30"/>
+    <col min="50" max="50" width="10.7109375" style="30" customWidth="1"/>
+    <col min="51" max="51" width="13.7109375" style="44" customWidth="1"/>
+    <col min="52" max="52" width="10.42578125" style="44" customWidth="1"/>
+    <col min="53" max="55" width="8.85546875" style="45"/>
+    <col min="56" max="56" width="10.7109375" style="45" customWidth="1"/>
+    <col min="57" max="57" width="13.7109375" style="46" customWidth="1"/>
+    <col min="58" max="58" width="10.42578125" style="46" customWidth="1"/>
+    <col min="59" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H1" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="13" t="s">
-        <v>114</v>
-      </c>
       <c r="K1" s="13" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>97</v>
+        <v>121</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>102</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="R1" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="T1" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="U1" s="15" t="s">
+      <c r="X1" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="W1" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="X1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z1" s="17" t="s">
-        <v>61</v>
+      <c r="Z1" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="AA1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC1" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD1" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC1" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD1" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE1" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="AF1" s="19" t="s">
-        <v>61</v>
+      <c r="AF1" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="AG1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI1" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ1" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="AH1" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="AI1" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ1" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK1" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="AL1" s="21" t="s">
-        <v>61</v>
+      <c r="AL1" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="AM1" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN1" s="22" t="s">
-        <v>116</v>
+        <v>60</v>
+      </c>
+      <c r="AN1" s="21" t="s">
+        <v>16</v>
       </c>
       <c r="AO1" s="22" t="s">
         <v>112</v>
       </c>
       <c r="AP1" s="22" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="AQ1" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="AR1" s="23" t="s">
-        <v>61</v>
+        <v>17</v>
+      </c>
+      <c r="AR1" s="22" t="s">
+        <v>94</v>
       </c>
       <c r="AS1" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU1" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="AV1" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="AT1" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="AU1" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="AV1" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="AW1" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AX1" s="25" t="s">
-        <v>61</v>
+      <c r="AX1" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="AY1" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="AZ1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA1" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="BB1" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="BC1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="AZ1" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="BA1" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="BB1" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="BC1" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="BD1" s="28" t="s">
-        <v>61</v>
+      <c r="BD1" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="BE1" s="28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="BF1" s="28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="30">
         <v>62</v>
@@ -2370,169 +2446,169 @@
         <v>1</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G2" s="31">
         <v>73</v>
       </c>
-      <c r="I2" s="32">
-        <v>1</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>100</v>
+      <c r="J2" s="32">
+        <v>1</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="34">
+        <v>34</v>
+      </c>
+      <c r="S2" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="K3" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="O2" s="34">
-        <v>34</v>
-      </c>
-      <c r="R2" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="J3" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="O3" s="34">
+      <c r="P3" s="34">
         <v>55</v>
       </c>
-      <c r="Q3" s="34">
+      <c r="R3" s="34">
         <v>18</v>
       </c>
-      <c r="R3" s="34">
-        <v>1</v>
-      </c>
-      <c r="T3" s="35">
+      <c r="S3" s="34">
+        <v>1</v>
+      </c>
+      <c r="U3" s="35">
         <v>1.5</v>
       </c>
-      <c r="U3" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="J4" s="33" t="s">
-        <v>99</v>
-      </c>
+      <c r="V3" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="K4" s="33" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="O4" s="34">
+        <v>86</v>
+      </c>
+      <c r="M4" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="P4" s="34">
         <v>36.587000000000003</v>
       </c>
-      <c r="Q4" s="34">
+      <c r="R4" s="34">
         <v>20</v>
       </c>
-      <c r="R4" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="S4" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
       <c r="D5" s="11">
         <v>2</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" s="31">
         <v>96</v>
       </c>
-      <c r="H5" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" s="32">
+      <c r="H5" s="31">
+        <v>16</v>
+      </c>
+      <c r="J5" s="32">
         <v>2</v>
       </c>
-      <c r="J5" s="33" t="s">
-        <v>107</v>
-      </c>
       <c r="K5" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="M5" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="N5" s="34">
+        <v>103</v>
+      </c>
+      <c r="L5" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="N5" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" s="34">
         <v>96</v>
       </c>
-      <c r="R5" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="S5" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
       <c r="D6" s="11">
         <v>3</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" s="31">
         <v>96</v>
       </c>
-      <c r="H6" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" s="32">
+      <c r="H6" s="31">
+        <v>16</v>
+      </c>
+      <c r="J6" s="32">
         <v>3</v>
       </c>
-      <c r="J6" s="33" t="s">
-        <v>107</v>
-      </c>
       <c r="K6" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="M6" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="N6" s="34">
+        <v>103</v>
+      </c>
+      <c r="L6" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="O6" s="34">
         <v>96</v>
       </c>
-      <c r="R6" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="J7" s="33" t="s">
-        <v>108</v>
-      </c>
+      <c r="S6" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
       <c r="K7" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="M7" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="N7" s="34">
+        <v>104</v>
+      </c>
+      <c r="L7" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="34">
         <v>96</v>
       </c>
-      <c r="R7" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="S7" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="30">
         <v>62</v>
@@ -2541,59 +2617,59 @@
         <v>1</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" s="31">
         <v>16</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="31">
+        <v>4</v>
+      </c>
+      <c r="J8" s="32">
+        <v>1</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="N8" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8" s="34">
+        <v>16</v>
+      </c>
+      <c r="S8" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="K9" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="L9" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="32">
-        <v>1</v>
-      </c>
-      <c r="J8" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="M8" s="34" t="s">
+      <c r="N9" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="34">
-        <v>16</v>
-      </c>
-      <c r="R8" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="J9" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="K9" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="L9" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="M9" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="O9" s="34">
+      <c r="P9" s="34">
         <v>9</v>
       </c>
-      <c r="R9" s="34">
+      <c r="S9" s="34">
         <v>0.85</v>
       </c>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="30" t="s">
         <v>68</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>69</v>
       </c>
       <c r="C10" s="30">
         <v>62</v>
@@ -2602,59 +2678,59 @@
         <v>1</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="31">
         <v>16</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="31">
+        <v>4</v>
+      </c>
+      <c r="J10" s="32">
+        <v>1</v>
+      </c>
+      <c r="K10" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="L10" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="N10" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O10" s="34">
+        <v>16</v>
+      </c>
+      <c r="S10" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="K11" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="L11" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="M11" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="32">
-        <v>1</v>
-      </c>
-      <c r="J10" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="K10" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="M10" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="N10" s="34">
-        <v>16</v>
-      </c>
-      <c r="R10" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="J11" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="K11" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="L11" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="M11" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="O11" s="34">
+      <c r="N11" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="34">
         <v>10</v>
       </c>
-      <c r="R11" s="34">
+      <c r="S11" s="34">
         <v>0.85</v>
       </c>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" s="30">
         <v>55</v>
@@ -2663,7 +2739,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F12" s="31">
         <v>54</v>
@@ -2671,102 +2747,102 @@
       <c r="H12" s="31">
         <v>9</v>
       </c>
-      <c r="I12" s="32">
-        <v>1</v>
-      </c>
-      <c r="J12" s="33" t="s">
-        <v>59</v>
+      <c r="J12" s="32">
+        <v>1</v>
       </c>
       <c r="K12" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="M12" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="N12" s="34">
+        <v>58</v>
+      </c>
+      <c r="L12" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="N12" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="O12" s="34">
         <v>54</v>
       </c>
-      <c r="R12" s="34">
+      <c r="S12" s="34">
         <v>0</v>
       </c>
-      <c r="T12" s="35">
+      <c r="U12" s="35">
         <v>0.3</v>
       </c>
-      <c r="U12" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="V12" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
       <c r="E13" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="J13" s="33" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="K13" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="L13" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="M13" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="O13" s="34">
+        <v>9</v>
+      </c>
+      <c r="S13" s="34">
+        <v>1</v>
+      </c>
+      <c r="W13" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="L13" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="M13" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="N13" s="34">
+      <c r="X13" s="36">
         <v>9</v>
       </c>
-      <c r="R13" s="34">
-        <v>1</v>
-      </c>
-      <c r="V13" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="W13" s="36">
+      <c r="Y13" s="36">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD13" s="38">
         <v>9</v>
       </c>
-      <c r="X13" s="36">
-        <v>1</v>
-      </c>
-      <c r="AB13" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC13" s="38">
+      <c r="AE13" s="38">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="40">
         <v>9</v>
       </c>
-      <c r="AD13" s="38">
-        <v>1</v>
-      </c>
-      <c r="AI13" s="40">
+      <c r="AK13" s="40">
+        <v>1</v>
+      </c>
+      <c r="AO13" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP13" s="42">
         <v>9</v>
       </c>
-      <c r="AJ13" s="40">
-        <v>1</v>
-      </c>
-      <c r="AN13" s="42" t="s">
-        <v>141</v>
-      </c>
-      <c r="AO13" s="42">
+      <c r="AQ13" s="42">
+        <v>1</v>
+      </c>
+      <c r="AU13" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="AV13" s="30">
         <v>9</v>
       </c>
-      <c r="AP13" s="42">
-        <v>1</v>
-      </c>
-      <c r="AT13" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="AU13" s="30">
-        <v>9</v>
-      </c>
-      <c r="AV13" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="AW13" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
       <c r="D14" s="11">
         <v>2</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F14" s="31">
         <v>54</v>
@@ -2774,102 +2850,102 @@
       <c r="H14" s="31">
         <v>9</v>
       </c>
-      <c r="I14" s="32">
-        <v>1</v>
-      </c>
-      <c r="J14" s="33" t="s">
-        <v>59</v>
+      <c r="J14" s="32">
+        <v>1</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="M14" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="N14" s="34">
+        <v>58</v>
+      </c>
+      <c r="L14" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="N14" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="O14" s="34">
         <v>54</v>
       </c>
-      <c r="R14" s="34">
+      <c r="S14" s="34">
         <v>0</v>
       </c>
-      <c r="T14" s="35">
+      <c r="U14" s="35">
         <v>0.3</v>
       </c>
-      <c r="U14" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="V14" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
       <c r="E15" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="J15" s="33" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="K15" s="33" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="L15" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="M15" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="N15" s="34">
+      <c r="M15" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="N15" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="O15" s="34">
         <v>9</v>
       </c>
-      <c r="R15" s="34">
-        <v>1</v>
-      </c>
-      <c r="V15" s="36" t="s">
-        <v>145</v>
-      </c>
-      <c r="W15" s="36">
+      <c r="S15" s="34">
+        <v>1</v>
+      </c>
+      <c r="W15" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="X15" s="36">
         <v>9</v>
       </c>
-      <c r="X15" s="36">
-        <v>1</v>
-      </c>
-      <c r="AB15" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC15" s="38">
+      <c r="Y15" s="36">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD15" s="38">
         <v>9</v>
       </c>
-      <c r="AD15" s="38">
-        <v>1</v>
-      </c>
-      <c r="AI15" s="40">
+      <c r="AE15" s="38">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="40">
         <v>9</v>
       </c>
-      <c r="AJ15" s="40">
-        <v>1</v>
-      </c>
-      <c r="AN15" s="42" t="s">
-        <v>147</v>
-      </c>
-      <c r="AO15" s="42">
+      <c r="AK15" s="40">
+        <v>1</v>
+      </c>
+      <c r="AO15" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="AP15" s="42">
         <v>9</v>
       </c>
-      <c r="AP15" s="42">
-        <v>1</v>
-      </c>
-      <c r="AT15" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="AU15" s="30">
+      <c r="AQ15" s="42">
+        <v>1</v>
+      </c>
+      <c r="AU15" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="AV15" s="30">
         <v>9</v>
       </c>
-      <c r="AV15" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="AW15" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:58" x14ac:dyDescent="0.3">
       <c r="D16" s="11">
         <v>3</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F16" s="31">
         <v>54</v>
@@ -2877,102 +2953,102 @@
       <c r="H16" s="31">
         <v>9</v>
       </c>
-      <c r="I16" s="32">
-        <v>1</v>
-      </c>
-      <c r="J16" s="33" t="s">
-        <v>59</v>
+      <c r="J16" s="32">
+        <v>1</v>
       </c>
       <c r="K16" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="M16" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="N16" s="34">
+        <v>58</v>
+      </c>
+      <c r="L16" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="N16" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="O16" s="34">
         <v>54</v>
       </c>
-      <c r="R16" s="34">
+      <c r="S16" s="34">
         <v>0</v>
       </c>
-      <c r="T16" s="35">
+      <c r="U16" s="35">
         <v>0.3</v>
       </c>
-      <c r="U16" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="4:48" x14ac:dyDescent="0.3">
+      <c r="V16" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:49" x14ac:dyDescent="0.3">
       <c r="E17" s="48" t="s">
-        <v>122</v>
-      </c>
-      <c r="J17" s="33" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="K17" s="33" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="L17" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="M17" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="N17" s="34">
+      <c r="M17" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="N17" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="O17" s="34">
         <v>9</v>
       </c>
-      <c r="R17" s="34">
-        <v>1</v>
-      </c>
-      <c r="V17" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="W17" s="36">
+      <c r="S17" s="34">
+        <v>1</v>
+      </c>
+      <c r="W17" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="X17" s="36">
         <v>9</v>
       </c>
-      <c r="X17" s="36">
-        <v>1</v>
-      </c>
-      <c r="AB17" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC17" s="38">
+      <c r="Y17" s="36">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD17" s="38">
         <v>9</v>
       </c>
-      <c r="AD17" s="38">
-        <v>1</v>
-      </c>
-      <c r="AI17" s="40">
+      <c r="AE17" s="38">
+        <v>1</v>
+      </c>
+      <c r="AJ17" s="40">
         <v>9</v>
       </c>
-      <c r="AJ17" s="40">
-        <v>1</v>
-      </c>
-      <c r="AN17" s="42" t="s">
-        <v>150</v>
-      </c>
-      <c r="AO17" s="42">
+      <c r="AK17" s="40">
+        <v>1</v>
+      </c>
+      <c r="AO17" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="AP17" s="42">
         <v>9</v>
       </c>
-      <c r="AP17" s="42">
-        <v>1</v>
-      </c>
-      <c r="AT17" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="AU17" s="30">
+      <c r="AQ17" s="42">
+        <v>1</v>
+      </c>
+      <c r="AU17" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="AV17" s="30">
         <v>9</v>
       </c>
-      <c r="AV17" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="4:48" x14ac:dyDescent="0.3">
+      <c r="AW17" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:49" x14ac:dyDescent="0.3">
       <c r="D18" s="11">
         <v>4</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F18" s="31">
         <v>54</v>
@@ -2980,58 +3056,58 @@
       <c r="H18" s="31">
         <v>9</v>
       </c>
-      <c r="I18" s="32">
-        <v>1</v>
-      </c>
-      <c r="J18" s="33" t="s">
-        <v>59</v>
+      <c r="J18" s="32">
+        <v>1</v>
       </c>
       <c r="K18" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="N18" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="O18" s="34">
+        <v>54</v>
+      </c>
+      <c r="S18" s="34">
+        <v>0</v>
+      </c>
+      <c r="U18" s="35">
+        <v>0.3</v>
+      </c>
+      <c r="V18" s="35">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="47"/>
+    </row>
+    <row r="19" spans="4:49" x14ac:dyDescent="0.3">
+      <c r="E19" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="M18" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="N18" s="34">
+      <c r="K19" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="L19" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="N19" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="O19" s="34">
         <v>54</v>
       </c>
-      <c r="R18" s="34">
-        <v>0</v>
-      </c>
-      <c r="T18" s="35">
-        <v>0.3</v>
-      </c>
-      <c r="U18" s="35">
-        <v>1</v>
-      </c>
-      <c r="AB18" s="47"/>
-    </row>
-    <row r="19" spans="4:48" x14ac:dyDescent="0.3">
-      <c r="E19" s="48" t="s">
-        <v>123</v>
-      </c>
-      <c r="J19" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="K19" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="M19" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="N19" s="34">
-        <v>54</v>
-      </c>
-      <c r="R19" s="34">
-        <v>1</v>
-      </c>
-      <c r="AB19" s="47"/>
-    </row>
-    <row r="26" spans="4:48" x14ac:dyDescent="0.3">
+      <c r="S19" s="34">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="47"/>
+    </row>
+    <row r="26" spans="4:49" x14ac:dyDescent="0.3">
       <c r="E26" s="49"/>
-      <c r="J26" s="50"/>
       <c r="K26" s="50"/>
       <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3059,33 +3135,33 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -3096,10 +3172,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -3110,10 +3186,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -3124,7 +3200,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -3160,34 +3236,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adds TODO list and documents minbeats/minseconds
</commit_message>
<xml_diff>
--- a/data/nott walking ex.2.xlsx
+++ b/data/nott walking ex.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="39255" yWindow="120" windowWidth="35100" windowHeight="18285" activeTab="2"/>
+    <workbookView xWindow="39255" yWindow="120" windowWidth="35100" windowHeight="18285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="175">
   <si>
     <t>theme</t>
   </si>
@@ -536,6 +536,18 @@
   </si>
   <si>
     <t>endeverybeats</t>
+  </si>
+  <si>
+    <t>minbeats</t>
+  </si>
+  <si>
+    <t>minseconds</t>
+  </si>
+  <si>
+    <t>test-t4-1</t>
+  </si>
+  <si>
+    <t>test-t4-2</t>
   </si>
 </sst>
 </file>
@@ -1761,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2179,6 +2191,52 @@
         <v>2</v>
       </c>
     </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="O15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="O16" s="8">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2192,10 +2250,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF26"/>
+  <dimension ref="A1:BH26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2206,57 +2264,57 @@
     <col min="4" max="4" width="8.85546875" style="11"/>
     <col min="5" max="5" width="22.140625" style="31" customWidth="1"/>
     <col min="6" max="6" width="7.140625" style="31" customWidth="1"/>
-    <col min="7" max="7" width="10" style="31" customWidth="1"/>
-    <col min="8" max="8" width="18" style="31" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="31" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="32" customWidth="1"/>
-    <col min="11" max="11" width="15" style="33" customWidth="1"/>
-    <col min="12" max="12" width="23" style="33" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="33" customWidth="1"/>
-    <col min="14" max="14" width="17" style="34" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="34" customWidth="1"/>
-    <col min="16" max="16" width="9" style="34" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" style="34" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" style="34" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" style="34" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" style="34" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" style="35" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" style="35" customWidth="1"/>
-    <col min="23" max="23" width="13.42578125" style="36" customWidth="1"/>
-    <col min="24" max="24" width="6.140625" style="36" customWidth="1"/>
-    <col min="25" max="25" width="9.85546875" style="36" customWidth="1"/>
-    <col min="26" max="26" width="10.7109375" style="36" customWidth="1"/>
-    <col min="27" max="27" width="13.7109375" style="37" customWidth="1"/>
-    <col min="28" max="28" width="10.42578125" style="37" customWidth="1"/>
-    <col min="29" max="29" width="17" style="38" customWidth="1"/>
-    <col min="30" max="30" width="6.140625" style="38" customWidth="1"/>
-    <col min="31" max="31" width="9.85546875" style="38" customWidth="1"/>
-    <col min="32" max="32" width="10.7109375" style="38" customWidth="1"/>
-    <col min="33" max="33" width="13.7109375" style="39" customWidth="1"/>
-    <col min="34" max="34" width="10.42578125" style="39" customWidth="1"/>
-    <col min="35" max="35" width="13.42578125" style="40" customWidth="1"/>
-    <col min="36" max="37" width="8.85546875" style="40"/>
-    <col min="38" max="38" width="10.7109375" style="40" customWidth="1"/>
-    <col min="39" max="39" width="13.7109375" style="41" customWidth="1"/>
-    <col min="40" max="40" width="10.42578125" style="41" customWidth="1"/>
-    <col min="41" max="41" width="14.85546875" style="42" customWidth="1"/>
-    <col min="42" max="43" width="8.85546875" style="42"/>
-    <col min="44" max="44" width="10.7109375" style="42" customWidth="1"/>
-    <col min="45" max="45" width="13.7109375" style="43" customWidth="1"/>
-    <col min="46" max="46" width="10.42578125" style="43" customWidth="1"/>
-    <col min="47" max="47" width="13.140625" style="30" customWidth="1"/>
-    <col min="48" max="49" width="8.85546875" style="30"/>
-    <col min="50" max="50" width="10.7109375" style="30" customWidth="1"/>
-    <col min="51" max="51" width="13.7109375" style="44" customWidth="1"/>
-    <col min="52" max="52" width="10.42578125" style="44" customWidth="1"/>
-    <col min="53" max="55" width="8.85546875" style="45"/>
-    <col min="56" max="56" width="10.7109375" style="45" customWidth="1"/>
-    <col min="57" max="57" width="13.7109375" style="46" customWidth="1"/>
-    <col min="58" max="58" width="10.42578125" style="46" customWidth="1"/>
-    <col min="59" max="16384" width="8.85546875" style="3"/>
+    <col min="7" max="9" width="10" style="31" customWidth="1"/>
+    <col min="10" max="10" width="18" style="31" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="31" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="32" customWidth="1"/>
+    <col min="13" max="13" width="15" style="33" customWidth="1"/>
+    <col min="14" max="14" width="23" style="33" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="33" customWidth="1"/>
+    <col min="16" max="16" width="17" style="34" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" style="34" customWidth="1"/>
+    <col min="18" max="18" width="9" style="34" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="34" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" style="34" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" style="34" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="34" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" style="35" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" style="35" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" style="36" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="36" customWidth="1"/>
+    <col min="27" max="27" width="9.85546875" style="36" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" style="36" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" style="37" customWidth="1"/>
+    <col min="30" max="30" width="10.42578125" style="37" customWidth="1"/>
+    <col min="31" max="31" width="17" style="38" customWidth="1"/>
+    <col min="32" max="32" width="6.140625" style="38" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" style="38" customWidth="1"/>
+    <col min="34" max="34" width="10.7109375" style="38" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="39" customWidth="1"/>
+    <col min="36" max="36" width="10.42578125" style="39" customWidth="1"/>
+    <col min="37" max="37" width="13.42578125" style="40" customWidth="1"/>
+    <col min="38" max="39" width="8.85546875" style="40"/>
+    <col min="40" max="40" width="10.7109375" style="40" customWidth="1"/>
+    <col min="41" max="41" width="13.7109375" style="41" customWidth="1"/>
+    <col min="42" max="42" width="10.42578125" style="41" customWidth="1"/>
+    <col min="43" max="43" width="14.85546875" style="42" customWidth="1"/>
+    <col min="44" max="45" width="8.85546875" style="42"/>
+    <col min="46" max="46" width="10.7109375" style="42" customWidth="1"/>
+    <col min="47" max="47" width="13.7109375" style="43" customWidth="1"/>
+    <col min="48" max="48" width="10.42578125" style="43" customWidth="1"/>
+    <col min="49" max="49" width="13.140625" style="30" customWidth="1"/>
+    <col min="50" max="51" width="8.85546875" style="30"/>
+    <col min="52" max="52" width="10.7109375" style="30" customWidth="1"/>
+    <col min="53" max="53" width="13.7109375" style="44" customWidth="1"/>
+    <col min="54" max="54" width="10.42578125" style="44" customWidth="1"/>
+    <col min="55" max="57" width="8.85546875" style="45"/>
+    <col min="58" max="58" width="10.7109375" style="45" customWidth="1"/>
+    <col min="59" max="59" width="13.7109375" style="46" customWidth="1"/>
+    <col min="60" max="60" width="10.42578125" style="46" customWidth="1"/>
+    <col min="61" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>100</v>
       </c>
@@ -2279,160 +2337,166 @@
         <v>109</v>
       </c>
       <c r="H1" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="T1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="U1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="V1" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="Y1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="Z1" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="Y1" s="16" t="s">
+      <c r="AA1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="16" t="s">
+      <c r="AB1" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="AA1" s="17" t="s">
+      <c r="AC1" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="AB1" s="17" t="s">
+      <c r="AD1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AE1" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AF1" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AG1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AH1" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AI1" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AJ1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AI1" s="20" t="s">
+      <c r="AK1" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="AJ1" s="20" t="s">
+      <c r="AL1" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="AK1" s="20" t="s">
+      <c r="AM1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="AL1" s="20" t="s">
+      <c r="AN1" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="AM1" s="21" t="s">
+      <c r="AO1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AN1" s="21" t="s">
+      <c r="AP1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="AO1" s="22" t="s">
+      <c r="AQ1" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="AP1" s="22" t="s">
+      <c r="AR1" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="AQ1" s="22" t="s">
+      <c r="AS1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="AR1" s="22" t="s">
+      <c r="AT1" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="AS1" s="23" t="s">
+      <c r="AU1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="AT1" s="23" t="s">
+      <c r="AV1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="AU1" s="24" t="s">
+      <c r="AW1" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="AV1" s="24" t="s">
+      <c r="AX1" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="AW1" s="24" t="s">
+      <c r="AY1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="AX1" s="10" t="s">
+      <c r="AZ1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="AY1" s="25" t="s">
+      <c r="BA1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="AZ1" s="25" t="s">
+      <c r="BB1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="BA1" s="26" t="s">
+      <c r="BC1" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="BB1" s="26" t="s">
+      <c r="BD1" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BC1" s="26" t="s">
+      <c r="BE1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="BD1" s="27" t="s">
+      <c r="BF1" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="BE1" s="28" t="s">
+      <c r="BG1" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="BF1" s="28" t="s">
+      <c r="BH1" s="28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>79</v>
       </c>
@@ -2451,78 +2515,81 @@
       <c r="G2" s="31">
         <v>73</v>
       </c>
-      <c r="J2" s="32">
-        <v>1</v>
-      </c>
-      <c r="K2" s="33" t="s">
+      <c r="I2" s="31">
+        <v>18</v>
+      </c>
+      <c r="L2" s="32">
+        <v>1</v>
+      </c>
+      <c r="M2" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="N2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="O2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="P2" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="P2" s="34">
+      <c r="R2" s="34">
         <v>34</v>
       </c>
-      <c r="S2" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="K3" s="33" t="s">
+      <c r="U2" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="M3" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="33" t="s">
+      <c r="N3" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="34" t="s">
+      <c r="P3" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="P3" s="34">
+      <c r="R3" s="34">
         <v>55</v>
       </c>
-      <c r="R3" s="34">
+      <c r="T3" s="34">
         <v>18</v>
       </c>
-      <c r="S3" s="34">
-        <v>1</v>
-      </c>
-      <c r="U3" s="35">
+      <c r="U3" s="34">
+        <v>1</v>
+      </c>
+      <c r="W3" s="35">
         <v>1.5</v>
       </c>
-      <c r="V3" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="K4" s="33" t="s">
+      <c r="X3" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="M4" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="N4" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="O4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="34" t="s">
+      <c r="P4" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="P4" s="34">
+      <c r="R4" s="34">
         <v>36.587000000000003</v>
       </c>
-      <c r="R4" s="34">
+      <c r="T4" s="34">
         <v>20</v>
       </c>
-      <c r="S4" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="U4" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
       <c r="D5" s="11">
         <v>2</v>
       </c>
@@ -2532,29 +2599,29 @@
       <c r="F5" s="31">
         <v>96</v>
       </c>
-      <c r="H5" s="31">
+      <c r="J5" s="31">
         <v>16</v>
       </c>
-      <c r="J5" s="32">
+      <c r="L5" s="32">
         <v>2</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="M5" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="33" t="s">
+      <c r="N5" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="N5" s="34" t="s">
+      <c r="P5" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="O5" s="34">
+      <c r="Q5" s="34">
         <v>96</v>
       </c>
-      <c r="S5" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="U5" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
       <c r="D6" s="11">
         <v>3</v>
       </c>
@@ -2564,46 +2631,46 @@
       <c r="F6" s="31">
         <v>96</v>
       </c>
-      <c r="H6" s="31">
+      <c r="J6" s="31">
         <v>16</v>
       </c>
-      <c r="J6" s="32">
+      <c r="L6" s="32">
         <v>3</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="M6" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="N6" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="N6" s="34" t="s">
+      <c r="P6" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="O6" s="34">
+      <c r="Q6" s="34">
         <v>96</v>
       </c>
-      <c r="S6" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="K7" s="33" t="s">
+      <c r="U6" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="M7" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="L7" s="33" t="s">
+      <c r="N7" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="34" t="s">
+      <c r="P7" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="O7" s="34">
+      <c r="Q7" s="34">
         <v>96</v>
       </c>
-      <c r="S7" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="U7" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
@@ -2622,49 +2689,49 @@
       <c r="F8" s="31">
         <v>16</v>
       </c>
-      <c r="H8" s="31">
+      <c r="J8" s="31">
         <v>4</v>
       </c>
-      <c r="J8" s="32">
-        <v>1</v>
-      </c>
-      <c r="K8" s="33" t="s">
+      <c r="L8" s="32">
+        <v>1</v>
+      </c>
+      <c r="M8" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="N8" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="N8" s="34" t="s">
+      <c r="P8" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="O8" s="34">
+      <c r="Q8" s="34">
         <v>16</v>
       </c>
-      <c r="S8" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="K9" s="33" t="s">
+      <c r="U8" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="M9" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="L9" s="33" t="s">
+      <c r="N9" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="M9" s="33" t="s">
+      <c r="O9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="N9" s="34" t="s">
+      <c r="P9" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P9" s="34">
+      <c r="R9" s="34">
         <v>9</v>
       </c>
-      <c r="S9" s="34">
+      <c r="U9" s="34">
         <v>0.85</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>67</v>
       </c>
@@ -2683,49 +2750,49 @@
       <c r="F10" s="31">
         <v>16</v>
       </c>
-      <c r="H10" s="31">
+      <c r="J10" s="31">
         <v>4</v>
       </c>
-      <c r="J10" s="32">
-        <v>1</v>
-      </c>
-      <c r="K10" s="33" t="s">
+      <c r="L10" s="32">
+        <v>1</v>
+      </c>
+      <c r="M10" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="N10" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="N10" s="34" t="s">
+      <c r="P10" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="O10" s="34">
+      <c r="Q10" s="34">
         <v>16</v>
       </c>
-      <c r="S10" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="K11" s="33" t="s">
+      <c r="U10" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="M11" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="L11" s="33" t="s">
+      <c r="N11" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="M11" s="33" t="s">
+      <c r="O11" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="N11" s="34" t="s">
+      <c r="P11" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="P11" s="34">
+      <c r="R11" s="34">
         <v>10</v>
       </c>
-      <c r="S11" s="34">
+      <c r="U11" s="34">
         <v>0.85</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>69</v>
       </c>
@@ -2744,100 +2811,100 @@
       <c r="F12" s="31">
         <v>54</v>
       </c>
-      <c r="H12" s="31">
+      <c r="J12" s="31">
         <v>9</v>
       </c>
-      <c r="J12" s="32">
-        <v>1</v>
-      </c>
-      <c r="K12" s="33" t="s">
+      <c r="L12" s="32">
+        <v>1</v>
+      </c>
+      <c r="M12" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="L12" s="33" t="s">
+      <c r="N12" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="N12" s="34" t="s">
+      <c r="P12" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="O12" s="34">
+      <c r="Q12" s="34">
         <v>54</v>
       </c>
-      <c r="S12" s="34">
+      <c r="U12" s="34">
         <v>0</v>
       </c>
-      <c r="U12" s="35">
+      <c r="W12" s="35">
         <v>0.3</v>
       </c>
-      <c r="V12" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="X12" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
       <c r="E13" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="K13" s="33" t="s">
+      <c r="M13" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="L13" s="33" t="s">
+      <c r="N13" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="M13" s="33" t="s">
+      <c r="O13" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="N13" s="34" t="s">
+      <c r="P13" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="O13" s="34">
+      <c r="Q13" s="34">
         <v>9</v>
       </c>
-      <c r="S13" s="34">
-        <v>1</v>
-      </c>
-      <c r="W13" s="36" t="s">
+      <c r="U13" s="34">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="X13" s="36">
+      <c r="Z13" s="36">
         <v>9</v>
       </c>
-      <c r="Y13" s="36">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="38" t="s">
+      <c r="AA13" s="36">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="AD13" s="38">
+      <c r="AF13" s="38">
         <v>9</v>
       </c>
-      <c r="AE13" s="38">
-        <v>1</v>
-      </c>
-      <c r="AJ13" s="40">
+      <c r="AG13" s="38">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="40">
         <v>9</v>
       </c>
-      <c r="AK13" s="40">
-        <v>1</v>
-      </c>
-      <c r="AO13" s="42" t="s">
+      <c r="AM13" s="40">
+        <v>1</v>
+      </c>
+      <c r="AQ13" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="AP13" s="42">
+      <c r="AR13" s="42">
         <v>9</v>
       </c>
-      <c r="AQ13" s="42">
-        <v>1</v>
-      </c>
-      <c r="AU13" s="30" t="s">
+      <c r="AS13" s="42">
+        <v>1</v>
+      </c>
+      <c r="AW13" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="AV13" s="30">
+      <c r="AX13" s="30">
         <v>9</v>
       </c>
-      <c r="AW13" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="AY13" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:60" x14ac:dyDescent="0.3">
       <c r="D14" s="11">
         <v>2</v>
       </c>
@@ -2847,100 +2914,100 @@
       <c r="F14" s="31">
         <v>54</v>
       </c>
-      <c r="H14" s="31">
+      <c r="J14" s="31">
         <v>9</v>
       </c>
-      <c r="J14" s="32">
-        <v>1</v>
-      </c>
-      <c r="K14" s="33" t="s">
+      <c r="L14" s="32">
+        <v>1</v>
+      </c>
+      <c r="M14" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="L14" s="33" t="s">
+      <c r="N14" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="N14" s="34" t="s">
+      <c r="P14" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="O14" s="34">
+      <c r="Q14" s="34">
         <v>54</v>
       </c>
-      <c r="S14" s="34">
+      <c r="U14" s="34">
         <v>0</v>
       </c>
-      <c r="U14" s="35">
+      <c r="W14" s="35">
         <v>0.3</v>
       </c>
-      <c r="V14" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="X14" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
       <c r="E15" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="K15" s="33" t="s">
+      <c r="M15" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="L15" s="33" t="s">
+      <c r="N15" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="M15" s="33" t="s">
+      <c r="O15" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="N15" s="34" t="s">
+      <c r="P15" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="O15" s="34">
+      <c r="Q15" s="34">
         <v>9</v>
       </c>
-      <c r="S15" s="34">
-        <v>1</v>
-      </c>
-      <c r="W15" s="36" t="s">
+      <c r="U15" s="34">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="X15" s="36">
+      <c r="Z15" s="36">
         <v>9</v>
       </c>
-      <c r="Y15" s="36">
-        <v>1</v>
-      </c>
-      <c r="AC15" s="47" t="s">
+      <c r="AA15" s="36">
+        <v>1</v>
+      </c>
+      <c r="AE15" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="AD15" s="38">
+      <c r="AF15" s="38">
         <v>9</v>
       </c>
-      <c r="AE15" s="38">
-        <v>1</v>
-      </c>
-      <c r="AJ15" s="40">
+      <c r="AG15" s="38">
+        <v>1</v>
+      </c>
+      <c r="AL15" s="40">
         <v>9</v>
       </c>
-      <c r="AK15" s="40">
-        <v>1</v>
-      </c>
-      <c r="AO15" s="42" t="s">
+      <c r="AM15" s="40">
+        <v>1</v>
+      </c>
+      <c r="AQ15" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="AP15" s="42">
+      <c r="AR15" s="42">
         <v>9</v>
       </c>
-      <c r="AQ15" s="42">
-        <v>1</v>
-      </c>
-      <c r="AU15" s="30" t="s">
+      <c r="AS15" s="42">
+        <v>1</v>
+      </c>
+      <c r="AW15" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="AV15" s="30">
+      <c r="AX15" s="30">
         <v>9</v>
       </c>
-      <c r="AW15" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="AY15" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:60" x14ac:dyDescent="0.3">
       <c r="D16" s="11">
         <v>3</v>
       </c>
@@ -2950,100 +3017,100 @@
       <c r="F16" s="31">
         <v>54</v>
       </c>
-      <c r="H16" s="31">
+      <c r="J16" s="31">
         <v>9</v>
       </c>
-      <c r="J16" s="32">
-        <v>1</v>
-      </c>
-      <c r="K16" s="33" t="s">
+      <c r="L16" s="32">
+        <v>1</v>
+      </c>
+      <c r="M16" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="N16" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="N16" s="34" t="s">
+      <c r="P16" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="O16" s="34">
+      <c r="Q16" s="34">
         <v>54</v>
       </c>
-      <c r="S16" s="34">
+      <c r="U16" s="34">
         <v>0</v>
       </c>
-      <c r="U16" s="35">
+      <c r="W16" s="35">
         <v>0.3</v>
       </c>
-      <c r="V16" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="4:49" x14ac:dyDescent="0.3">
+      <c r="X16" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:51" x14ac:dyDescent="0.3">
       <c r="E17" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="K17" s="33" t="s">
+      <c r="M17" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="L17" s="33" t="s">
+      <c r="N17" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="M17" s="33" t="s">
+      <c r="O17" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="N17" s="34" t="s">
+      <c r="P17" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="O17" s="34">
+      <c r="Q17" s="34">
         <v>9</v>
       </c>
-      <c r="S17" s="34">
-        <v>1</v>
-      </c>
-      <c r="W17" s="36" t="s">
+      <c r="U17" s="34">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="X17" s="36">
+      <c r="Z17" s="36">
         <v>9</v>
       </c>
-      <c r="Y17" s="36">
-        <v>1</v>
-      </c>
-      <c r="AC17" s="47" t="s">
+      <c r="AA17" s="36">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="AD17" s="38">
+      <c r="AF17" s="38">
         <v>9</v>
       </c>
-      <c r="AE17" s="38">
-        <v>1</v>
-      </c>
-      <c r="AJ17" s="40">
+      <c r="AG17" s="38">
+        <v>1</v>
+      </c>
+      <c r="AL17" s="40">
         <v>9</v>
       </c>
-      <c r="AK17" s="40">
-        <v>1</v>
-      </c>
-      <c r="AO17" s="42" t="s">
+      <c r="AM17" s="40">
+        <v>1</v>
+      </c>
+      <c r="AQ17" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="AP17" s="42">
+      <c r="AR17" s="42">
         <v>9</v>
       </c>
-      <c r="AQ17" s="42">
-        <v>1</v>
-      </c>
-      <c r="AU17" s="30" t="s">
+      <c r="AS17" s="42">
+        <v>1</v>
+      </c>
+      <c r="AW17" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="AV17" s="30">
+      <c r="AX17" s="30">
         <v>9</v>
       </c>
-      <c r="AW17" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="4:49" x14ac:dyDescent="0.3">
+      <c r="AY17" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:51" x14ac:dyDescent="0.3">
       <c r="D18" s="11">
         <v>4</v>
       </c>
@@ -3053,61 +3120,61 @@
       <c r="F18" s="31">
         <v>54</v>
       </c>
-      <c r="H18" s="31">
+      <c r="J18" s="31">
         <v>9</v>
       </c>
-      <c r="J18" s="32">
-        <v>1</v>
-      </c>
-      <c r="K18" s="33" t="s">
+      <c r="L18" s="32">
+        <v>1</v>
+      </c>
+      <c r="M18" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="L18" s="33" t="s">
+      <c r="N18" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="N18" s="34" t="s">
+      <c r="P18" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="O18" s="34">
+      <c r="Q18" s="34">
         <v>54</v>
       </c>
-      <c r="S18" s="34">
+      <c r="U18" s="34">
         <v>0</v>
       </c>
-      <c r="U18" s="35">
+      <c r="W18" s="35">
         <v>0.3</v>
       </c>
-      <c r="V18" s="35">
-        <v>1</v>
-      </c>
-      <c r="AC18" s="47"/>
-    </row>
-    <row r="19" spans="4:49" x14ac:dyDescent="0.3">
+      <c r="X18" s="35">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="47"/>
+    </row>
+    <row r="19" spans="4:51" x14ac:dyDescent="0.3">
       <c r="E19" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="K19" s="33" t="s">
+      <c r="M19" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="L19" s="33" t="s">
+      <c r="N19" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="N19" s="34" t="s">
+      <c r="P19" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="O19" s="34">
+      <c r="Q19" s="34">
         <v>54</v>
       </c>
-      <c r="S19" s="34">
-        <v>1</v>
-      </c>
-      <c r="AC19" s="47"/>
-    </row>
-    <row r="26" spans="4:49" x14ac:dyDescent="0.3">
+      <c r="U19" s="34">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="47"/>
+    </row>
+    <row r="26" spans="4:51" x14ac:dyDescent="0.3">
       <c r="E26" s="49"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="50"/>
       <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds support for minbeats/minseconds
</commit_message>
<xml_diff>
--- a/data/nott walking ex.2.xlsx
+++ b/data/nott walking ex.2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26330"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="39255" yWindow="120" windowWidth="35100" windowHeight="18285" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="176">
   <si>
     <t>theme</t>
   </si>
@@ -548,6 +548,9 @@
   </si>
   <si>
     <t>test-t4-2</t>
+  </si>
+  <si>
+    <t>test-t1-1</t>
   </si>
 </sst>
 </file>
@@ -737,8 +740,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="247">
+  <cellStyleXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1135,7 +1140,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="247">
+  <cellStyles count="249">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1259,6 +1264,7 @@
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1382,6 +1388,7 @@
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1440,7 +1447,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1475,7 +1482,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1690,13 +1697,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1704,7 +1711,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1712,7 +1719,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1720,7 +1727,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1728,7 +1735,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1736,7 +1743,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1744,7 +1751,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1752,7 +1759,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -1773,33 +1780,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="11.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="16" style="3" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="34.7109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="8" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" style="8" customWidth="1"/>
+    <col min="12" max="12" width="22.5" style="3" customWidth="1"/>
+    <col min="13" max="13" width="34.6640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="8.1640625" style="8" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" style="8" customWidth="1"/>
     <col min="16" max="16" width="12" style="3" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" style="3"/>
+    <col min="17" max="17" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="2" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>33</v>
       </c>
@@ -1850,7 +1857,7 @@
       </c>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17">
       <c r="B2" s="3" t="s">
         <v>92</v>
       </c>
@@ -1876,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17">
       <c r="B3" s="3" t="s">
         <v>157</v>
       </c>
@@ -1899,7 +1906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="29">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1931,7 +1938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="29">
       <c r="B5" s="3" t="s">
         <v>89</v>
       </c>
@@ -1960,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="45.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="43">
       <c r="A6" s="9">
         <v>2</v>
       </c>
@@ -1992,7 +1999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="45.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="43">
       <c r="A7" s="9">
         <v>3</v>
       </c>
@@ -2024,7 +2031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17">
       <c r="A8" s="9">
         <v>4</v>
       </c>
@@ -2053,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17">
       <c r="B9" s="6" t="s">
         <v>81</v>
       </c>
@@ -2079,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17">
       <c r="B10" s="6" t="s">
         <v>81</v>
       </c>
@@ -2105,7 +2112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17">
       <c r="B11" s="6" t="s">
         <v>81</v>
       </c>
@@ -2131,12 +2138,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17">
       <c r="A12" s="9" t="s">
         <v>166</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>35</v>
@@ -2151,15 +2158,15 @@
         <v>79</v>
       </c>
       <c r="O12" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="9" t="s">
         <v>166</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>35</v>
@@ -2174,52 +2181,52 @@
         <v>79</v>
       </c>
       <c r="O13" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="9" t="s">
         <v>166</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="O14" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="9" t="s">
         <v>166</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I15" s="3">
-        <v>1</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="O15" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="9" t="s">
         <v>166</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>35</v>
@@ -2234,6 +2241,29 @@
         <v>69</v>
       </c>
       <c r="O16" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="O17" s="8">
         <v>2</v>
       </c>
     </row>
@@ -2256,65 +2286,65 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="10"/>
-    <col min="2" max="2" width="31.7109375" style="30" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="30"/>
-    <col min="4" max="4" width="8.85546875" style="11"/>
-    <col min="5" max="5" width="22.140625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="10"/>
+    <col min="2" max="2" width="31.6640625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="30"/>
+    <col min="4" max="4" width="8.83203125" style="11"/>
+    <col min="5" max="5" width="22.1640625" style="31" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" style="31" customWidth="1"/>
     <col min="7" max="9" width="10" style="31" customWidth="1"/>
     <col min="10" max="10" width="18" style="31" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="31" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="32" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="31" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="32" customWidth="1"/>
     <col min="13" max="13" width="15" style="33" customWidth="1"/>
     <col min="14" max="14" width="23" style="33" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="33" customWidth="1"/>
+    <col min="15" max="15" width="13.5" style="33" customWidth="1"/>
     <col min="16" max="16" width="17" style="34" customWidth="1"/>
-    <col min="17" max="17" width="6.7109375" style="34" customWidth="1"/>
+    <col min="17" max="17" width="6.6640625" style="34" customWidth="1"/>
     <col min="18" max="18" width="9" style="34" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="34" customWidth="1"/>
-    <col min="20" max="20" width="14.7109375" style="34" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" style="34" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" style="34" customWidth="1"/>
-    <col min="23" max="23" width="13.7109375" style="35" customWidth="1"/>
-    <col min="24" max="24" width="10.42578125" style="35" customWidth="1"/>
-    <col min="25" max="25" width="13.42578125" style="36" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" style="36" customWidth="1"/>
-    <col min="27" max="27" width="9.85546875" style="36" customWidth="1"/>
-    <col min="28" max="28" width="10.7109375" style="36" customWidth="1"/>
-    <col min="29" max="29" width="13.7109375" style="37" customWidth="1"/>
-    <col min="30" max="30" width="10.42578125" style="37" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="34" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" style="34" customWidth="1"/>
+    <col min="21" max="21" width="9.83203125" style="34" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" style="34" customWidth="1"/>
+    <col min="23" max="23" width="13.6640625" style="35" customWidth="1"/>
+    <col min="24" max="24" width="10.5" style="35" customWidth="1"/>
+    <col min="25" max="25" width="13.5" style="36" customWidth="1"/>
+    <col min="26" max="26" width="6.1640625" style="36" customWidth="1"/>
+    <col min="27" max="27" width="9.83203125" style="36" customWidth="1"/>
+    <col min="28" max="28" width="10.6640625" style="36" customWidth="1"/>
+    <col min="29" max="29" width="13.6640625" style="37" customWidth="1"/>
+    <col min="30" max="30" width="10.5" style="37" customWidth="1"/>
     <col min="31" max="31" width="17" style="38" customWidth="1"/>
-    <col min="32" max="32" width="6.140625" style="38" customWidth="1"/>
-    <col min="33" max="33" width="9.85546875" style="38" customWidth="1"/>
-    <col min="34" max="34" width="10.7109375" style="38" customWidth="1"/>
-    <col min="35" max="35" width="13.7109375" style="39" customWidth="1"/>
-    <col min="36" max="36" width="10.42578125" style="39" customWidth="1"/>
-    <col min="37" max="37" width="13.42578125" style="40" customWidth="1"/>
-    <col min="38" max="39" width="8.85546875" style="40"/>
-    <col min="40" max="40" width="10.7109375" style="40" customWidth="1"/>
-    <col min="41" max="41" width="13.7109375" style="41" customWidth="1"/>
-    <col min="42" max="42" width="10.42578125" style="41" customWidth="1"/>
-    <col min="43" max="43" width="14.85546875" style="42" customWidth="1"/>
-    <col min="44" max="45" width="8.85546875" style="42"/>
-    <col min="46" max="46" width="10.7109375" style="42" customWidth="1"/>
-    <col min="47" max="47" width="13.7109375" style="43" customWidth="1"/>
-    <col min="48" max="48" width="10.42578125" style="43" customWidth="1"/>
-    <col min="49" max="49" width="13.140625" style="30" customWidth="1"/>
-    <col min="50" max="51" width="8.85546875" style="30"/>
-    <col min="52" max="52" width="10.7109375" style="30" customWidth="1"/>
-    <col min="53" max="53" width="13.7109375" style="44" customWidth="1"/>
-    <col min="54" max="54" width="10.42578125" style="44" customWidth="1"/>
-    <col min="55" max="57" width="8.85546875" style="45"/>
-    <col min="58" max="58" width="10.7109375" style="45" customWidth="1"/>
-    <col min="59" max="59" width="13.7109375" style="46" customWidth="1"/>
-    <col min="60" max="60" width="10.42578125" style="46" customWidth="1"/>
-    <col min="61" max="16384" width="8.85546875" style="3"/>
+    <col min="32" max="32" width="6.1640625" style="38" customWidth="1"/>
+    <col min="33" max="33" width="9.83203125" style="38" customWidth="1"/>
+    <col min="34" max="34" width="10.6640625" style="38" customWidth="1"/>
+    <col min="35" max="35" width="13.6640625" style="39" customWidth="1"/>
+    <col min="36" max="36" width="10.5" style="39" customWidth="1"/>
+    <col min="37" max="37" width="13.5" style="40" customWidth="1"/>
+    <col min="38" max="39" width="8.83203125" style="40"/>
+    <col min="40" max="40" width="10.6640625" style="40" customWidth="1"/>
+    <col min="41" max="41" width="13.6640625" style="41" customWidth="1"/>
+    <col min="42" max="42" width="10.5" style="41" customWidth="1"/>
+    <col min="43" max="43" width="14.83203125" style="42" customWidth="1"/>
+    <col min="44" max="45" width="8.83203125" style="42"/>
+    <col min="46" max="46" width="10.6640625" style="42" customWidth="1"/>
+    <col min="47" max="47" width="13.6640625" style="43" customWidth="1"/>
+    <col min="48" max="48" width="10.5" style="43" customWidth="1"/>
+    <col min="49" max="49" width="13.1640625" style="30" customWidth="1"/>
+    <col min="50" max="51" width="8.83203125" style="30"/>
+    <col min="52" max="52" width="10.6640625" style="30" customWidth="1"/>
+    <col min="53" max="53" width="13.6640625" style="44" customWidth="1"/>
+    <col min="54" max="54" width="10.5" style="44" customWidth="1"/>
+    <col min="55" max="57" width="8.83203125" style="45"/>
+    <col min="58" max="58" width="10.6640625" style="45" customWidth="1"/>
+    <col min="59" max="59" width="13.6640625" style="46" customWidth="1"/>
+    <col min="60" max="60" width="10.5" style="46" customWidth="1"/>
+    <col min="61" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" s="8" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>100</v>
       </c>
@@ -2496,7 +2526,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60">
       <c r="A2" s="10" t="s">
         <v>79</v>
       </c>
@@ -2516,7 +2546,7 @@
         <v>73</v>
       </c>
       <c r="I2" s="31">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="L2" s="32">
         <v>1</v>
@@ -2540,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60">
       <c r="M3" s="33" t="s">
         <v>58</v>
       </c>
@@ -2566,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60">
       <c r="M4" s="33" t="s">
         <v>95</v>
       </c>
@@ -2589,7 +2619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60">
       <c r="D5" s="11">
         <v>2</v>
       </c>
@@ -2621,7 +2651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60">
       <c r="D6" s="11">
         <v>3</v>
       </c>
@@ -2653,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60">
       <c r="M7" s="33" t="s">
         <v>104</v>
       </c>
@@ -2670,7 +2700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60">
       <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
@@ -2711,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:60">
       <c r="M9" s="33" t="s">
         <v>96</v>
       </c>
@@ -2731,7 +2761,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:60">
       <c r="A10" s="10" t="s">
         <v>67</v>
       </c>
@@ -2772,7 +2802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:60">
       <c r="M11" s="33" t="s">
         <v>106</v>
       </c>
@@ -2792,7 +2822,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:60">
       <c r="A12" s="10" t="s">
         <v>69</v>
       </c>
@@ -2839,7 +2869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:60">
       <c r="E13" s="31" t="s">
         <v>116</v>
       </c>
@@ -2904,7 +2934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:60">
       <c r="D14" s="11">
         <v>2</v>
       </c>
@@ -2942,7 +2972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:60">
       <c r="E15" s="31" t="s">
         <v>117</v>
       </c>
@@ -3007,7 +3037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:60">
       <c r="D16" s="11">
         <v>3</v>
       </c>
@@ -3045,7 +3075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:51" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:51">
       <c r="E17" s="48" t="s">
         <v>118</v>
       </c>
@@ -3110,7 +3140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="4:51" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:51">
       <c r="D18" s="11">
         <v>4</v>
       </c>
@@ -3149,7 +3179,7 @@
       </c>
       <c r="AE18" s="47"/>
     </row>
-    <row r="19" spans="4:51" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:51">
       <c r="E19" s="48" t="s">
         <v>119</v>
       </c>
@@ -3170,7 +3200,7 @@
       </c>
       <c r="AE19" s="47"/>
     </row>
-    <row r="26" spans="4:51" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:51">
       <c r="E26" s="49"/>
       <c r="M26" s="50"/>
       <c r="N26" s="50"/>
@@ -3195,12 +3225,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3223,7 +3253,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3237,7 +3267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3251,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -3265,7 +3295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -3289,19 +3319,19 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
     <col min="3" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -3333,7 +3363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3350,7 +3380,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3367,7 +3397,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3384,7 +3414,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3401,7 +3431,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
adds support for file volumes and fades
</commit_message>
<xml_diff>
--- a/data/nott walking ex.2.xlsx
+++ b/data/nott walking ex.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26330"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -1782,7 +1782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
@@ -2282,8 +2282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2567,6 +2567,12 @@
         <v>34</v>
       </c>
       <c r="U2" s="34">
+        <v>0.2</v>
+      </c>
+      <c r="W2" s="35">
+        <v>4</v>
+      </c>
+      <c r="X2" s="35">
         <v>1</v>
       </c>
     </row>
@@ -2587,13 +2593,13 @@
         <v>18</v>
       </c>
       <c r="U3" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3" s="35">
         <v>1.5</v>
       </c>
       <c r="X3" s="35">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:60">
@@ -2680,7 +2686,7 @@
         <v>96</v>
       </c>
       <c r="U6" s="34">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:60">
@@ -2866,7 +2872,7 @@
         <v>0.3</v>
       </c>
       <c r="X12" s="35">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:60">

</xml_diff>

<commit_message>
adds short fade at end of file
</commit_message>
<xml_diff>
--- a/data/nott walking ex.2.xlsx
+++ b/data/nott walking ex.2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26330"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25365" windowHeight="15285" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="179">
   <si>
     <t>theme</t>
   </si>
@@ -551,6 +551,15 @@
   </si>
   <si>
     <t>test-t1-1</t>
+  </si>
+  <si>
+    <t>glitch</t>
+  </si>
+  <si>
+    <t>Glitch test</t>
+  </si>
+  <si>
+    <t>bit of piano</t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1456,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1482,7 +1491,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1697,13 +1706,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1711,7 +1720,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1719,7 +1728,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1727,7 +1736,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1735,7 +1744,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1743,7 +1752,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1751,7 +1760,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1759,7 +1768,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -1780,33 +1789,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="4.83203125" style="3" customWidth="1"/>
-    <col min="5" max="6" width="11.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="3" customWidth="1"/>
     <col min="11" max="11" width="16" style="3" customWidth="1"/>
-    <col min="12" max="12" width="22.5" style="3" customWidth="1"/>
-    <col min="13" max="13" width="34.6640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="8.1640625" style="8" customWidth="1"/>
-    <col min="15" max="15" width="18.6640625" style="8" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="34.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="8" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" style="8" customWidth="1"/>
     <col min="16" max="16" width="12" style="3" customWidth="1"/>
-    <col min="17" max="17" width="8.83203125" style="3"/>
+    <col min="17" max="17" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1">
+    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>33</v>
       </c>
@@ -1857,7 +1866,7 @@
       </c>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>92</v>
       </c>
@@ -1883,7 +1892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>157</v>
       </c>
@@ -1906,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="29">
+    <row r="4" spans="1:17" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1938,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="29">
+    <row r="5" spans="1:17" ht="30.75" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>89</v>
       </c>
@@ -1967,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="43">
+    <row r="6" spans="1:17" ht="45.75" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>2</v>
       </c>
@@ -1999,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="43">
+    <row r="7" spans="1:17" ht="45.75" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>3</v>
       </c>
@@ -2031,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>4</v>
       </c>
@@ -2060,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>81</v>
       </c>
@@ -2086,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>81</v>
       </c>
@@ -2112,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>81</v>
       </c>
@@ -2138,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>166</v>
       </c>
@@ -2161,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>166</v>
       </c>
@@ -2184,7 +2193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>166</v>
       </c>
@@ -2207,7 +2216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>166</v>
       </c>
@@ -2221,7 +2230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>166</v>
       </c>
@@ -2244,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>166</v>
       </c>
@@ -2265,6 +2274,26 @@
       </c>
       <c r="O17" s="8">
         <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="O18" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2282,69 +2311,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="10"/>
-    <col min="2" max="2" width="31.6640625" style="30" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="30"/>
-    <col min="4" max="4" width="8.83203125" style="11"/>
-    <col min="5" max="5" width="22.1640625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="10"/>
+    <col min="2" max="2" width="31.7109375" style="30" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="30"/>
+    <col min="4" max="4" width="8.85546875" style="11"/>
+    <col min="5" max="5" width="22.140625" style="31" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="31" customWidth="1"/>
     <col min="7" max="9" width="10" style="31" customWidth="1"/>
     <col min="10" max="10" width="18" style="31" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="31" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="32" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="31" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="32" customWidth="1"/>
     <col min="13" max="13" width="15" style="33" customWidth="1"/>
     <col min="14" max="14" width="23" style="33" customWidth="1"/>
-    <col min="15" max="15" width="13.5" style="33" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="33" customWidth="1"/>
     <col min="16" max="16" width="17" style="34" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" style="34" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" style="34" customWidth="1"/>
     <col min="18" max="18" width="9" style="34" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" style="34" customWidth="1"/>
-    <col min="20" max="20" width="14.6640625" style="34" customWidth="1"/>
-    <col min="21" max="21" width="9.83203125" style="34" customWidth="1"/>
-    <col min="22" max="22" width="10.6640625" style="34" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" style="35" customWidth="1"/>
-    <col min="24" max="24" width="10.5" style="35" customWidth="1"/>
-    <col min="25" max="25" width="13.5" style="36" customWidth="1"/>
-    <col min="26" max="26" width="6.1640625" style="36" customWidth="1"/>
-    <col min="27" max="27" width="9.83203125" style="36" customWidth="1"/>
-    <col min="28" max="28" width="10.6640625" style="36" customWidth="1"/>
-    <col min="29" max="29" width="13.6640625" style="37" customWidth="1"/>
-    <col min="30" max="30" width="10.5" style="37" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="34" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" style="34" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" style="34" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="34" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" style="35" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" style="35" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" style="36" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="36" customWidth="1"/>
+    <col min="27" max="27" width="9.85546875" style="36" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" style="36" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" style="37" customWidth="1"/>
+    <col min="30" max="30" width="10.42578125" style="37" customWidth="1"/>
     <col min="31" max="31" width="17" style="38" customWidth="1"/>
-    <col min="32" max="32" width="6.1640625" style="38" customWidth="1"/>
-    <col min="33" max="33" width="9.83203125" style="38" customWidth="1"/>
-    <col min="34" max="34" width="10.6640625" style="38" customWidth="1"/>
-    <col min="35" max="35" width="13.6640625" style="39" customWidth="1"/>
-    <col min="36" max="36" width="10.5" style="39" customWidth="1"/>
-    <col min="37" max="37" width="13.5" style="40" customWidth="1"/>
-    <col min="38" max="39" width="8.83203125" style="40"/>
-    <col min="40" max="40" width="10.6640625" style="40" customWidth="1"/>
-    <col min="41" max="41" width="13.6640625" style="41" customWidth="1"/>
-    <col min="42" max="42" width="10.5" style="41" customWidth="1"/>
-    <col min="43" max="43" width="14.83203125" style="42" customWidth="1"/>
-    <col min="44" max="45" width="8.83203125" style="42"/>
-    <col min="46" max="46" width="10.6640625" style="42" customWidth="1"/>
-    <col min="47" max="47" width="13.6640625" style="43" customWidth="1"/>
-    <col min="48" max="48" width="10.5" style="43" customWidth="1"/>
-    <col min="49" max="49" width="13.1640625" style="30" customWidth="1"/>
-    <col min="50" max="51" width="8.83203125" style="30"/>
-    <col min="52" max="52" width="10.6640625" style="30" customWidth="1"/>
-    <col min="53" max="53" width="13.6640625" style="44" customWidth="1"/>
-    <col min="54" max="54" width="10.5" style="44" customWidth="1"/>
-    <col min="55" max="57" width="8.83203125" style="45"/>
-    <col min="58" max="58" width="10.6640625" style="45" customWidth="1"/>
-    <col min="59" max="59" width="13.6640625" style="46" customWidth="1"/>
-    <col min="60" max="60" width="10.5" style="46" customWidth="1"/>
-    <col min="61" max="16384" width="8.83203125" style="3"/>
+    <col min="32" max="32" width="6.140625" style="38" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" style="38" customWidth="1"/>
+    <col min="34" max="34" width="10.7109375" style="38" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="39" customWidth="1"/>
+    <col min="36" max="36" width="10.42578125" style="39" customWidth="1"/>
+    <col min="37" max="37" width="13.42578125" style="40" customWidth="1"/>
+    <col min="38" max="39" width="8.85546875" style="40"/>
+    <col min="40" max="40" width="10.7109375" style="40" customWidth="1"/>
+    <col min="41" max="41" width="13.7109375" style="41" customWidth="1"/>
+    <col min="42" max="42" width="10.42578125" style="41" customWidth="1"/>
+    <col min="43" max="43" width="14.85546875" style="42" customWidth="1"/>
+    <col min="44" max="45" width="8.85546875" style="42"/>
+    <col min="46" max="46" width="10.7109375" style="42" customWidth="1"/>
+    <col min="47" max="47" width="13.7109375" style="43" customWidth="1"/>
+    <col min="48" max="48" width="10.42578125" style="43" customWidth="1"/>
+    <col min="49" max="49" width="13.140625" style="30" customWidth="1"/>
+    <col min="50" max="51" width="8.85546875" style="30"/>
+    <col min="52" max="52" width="10.7109375" style="30" customWidth="1"/>
+    <col min="53" max="53" width="13.7109375" style="44" customWidth="1"/>
+    <col min="54" max="54" width="10.42578125" style="44" customWidth="1"/>
+    <col min="55" max="57" width="8.85546875" style="45"/>
+    <col min="58" max="58" width="10.7109375" style="45" customWidth="1"/>
+    <col min="59" max="59" width="13.7109375" style="46" customWidth="1"/>
+    <col min="60" max="60" width="10.42578125" style="46" customWidth="1"/>
+    <col min="61" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" s="8" customFormat="1">
+    <row r="1" spans="1:60" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>100</v>
       </c>
@@ -2526,7 +2555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:60">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>79</v>
       </c>
@@ -2576,7 +2605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:60">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="M3" s="33" t="s">
         <v>58</v>
       </c>
@@ -2602,7 +2631,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:60">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="M4" s="33" t="s">
         <v>95</v>
       </c>
@@ -2625,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:60">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
       <c r="D5" s="11">
         <v>2</v>
       </c>
@@ -2657,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:60">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
       <c r="D6" s="11">
         <v>3</v>
       </c>
@@ -2689,7 +2718,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:60">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
       <c r="M7" s="33" t="s">
         <v>104</v>
       </c>
@@ -2706,7 +2735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:60">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
@@ -2747,7 +2776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:60">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
       <c r="M9" s="33" t="s">
         <v>96</v>
       </c>
@@ -2767,7 +2796,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="10" spans="1:60">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>67</v>
       </c>
@@ -2808,7 +2837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:60">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
       <c r="M11" s="33" t="s">
         <v>106</v>
       </c>
@@ -2828,7 +2857,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="12" spans="1:60">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>69</v>
       </c>
@@ -2875,7 +2904,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:60">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
       <c r="E13" s="31" t="s">
         <v>116</v>
       </c>
@@ -2940,7 +2969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:60">
+    <row r="14" spans="1:60" x14ac:dyDescent="0.3">
       <c r="D14" s="11">
         <v>2</v>
       </c>
@@ -2978,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:60">
+    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
       <c r="E15" s="31" t="s">
         <v>117</v>
       </c>
@@ -3043,7 +3072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:60">
+    <row r="16" spans="1:60" x14ac:dyDescent="0.3">
       <c r="D16" s="11">
         <v>3</v>
       </c>
@@ -3081,7 +3110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:51">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.3">
       <c r="E17" s="48" t="s">
         <v>118</v>
       </c>
@@ -3146,7 +3175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="4:51">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.3">
       <c r="D18" s="11">
         <v>4</v>
       </c>
@@ -3185,7 +3214,7 @@
       </c>
       <c r="AE18" s="47"/>
     </row>
-    <row r="19" spans="4:51">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.3">
       <c r="E19" s="48" t="s">
         <v>119</v>
       </c>
@@ -3206,7 +3235,42 @@
       </c>
       <c r="AE19" s="47"/>
     </row>
-    <row r="26" spans="4:51">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="30">
+        <v>55</v>
+      </c>
+      <c r="D20" s="11">
+        <v>1</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="F20" s="31">
+        <v>3</v>
+      </c>
+      <c r="J20" s="31">
+        <v>1</v>
+      </c>
+      <c r="L20" s="32">
+        <v>1</v>
+      </c>
+      <c r="M20" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="P20" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q20" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:51" x14ac:dyDescent="0.3">
       <c r="E26" s="49"/>
       <c r="M26" s="50"/>
       <c r="N26" s="50"/>
@@ -3231,12 +3295,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3259,7 +3323,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3273,7 +3337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3287,7 +3351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -3301,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -3325,19 +3389,19 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -3369,7 +3433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3386,7 +3450,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3403,7 +3467,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3420,7 +3484,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3437,7 +3501,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
support basic theme transitions (fade out)
</commit_message>
<xml_diff>
--- a/data/nott walking ex.2.xlsx
+++ b/data/nott walking ex.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26330"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="177">
   <si>
     <t>theme</t>
   </si>
@@ -67,12 +67,6 @@
     <t>fromtheme</t>
   </si>
   <si>
-    <t>totheme</t>
-  </si>
-  <si>
-    <t>sync? (may not be supported)</t>
-  </si>
-  <si>
     <t>volume2</t>
   </si>
   <si>
@@ -85,16 +79,7 @@
     <t>delayseconds</t>
   </si>
   <si>
-    <t>fadeinseconds</t>
-  </si>
-  <si>
     <t>tempo</t>
-  </si>
-  <si>
-    <t>fromlevel</t>
-  </si>
-  <si>
-    <t>tolevel</t>
   </si>
   <si>
     <t>priority</t>
@@ -758,8 +743,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="257">
+  <cellStyleXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1166,7 +1153,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="257">
+  <cellStyles count="259">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1295,6 +1282,7 @@
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1423,6 +1411,7 @@
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1739,26 +1728,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1766,39 +1755,39 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1844,49 +1833,49 @@
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1">
       <c r="A1" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>0</v>
@@ -1895,28 +1884,28 @@
         <v>3</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="S1" s="4"/>
     </row>
     <row r="2" spans="1:19">
       <c r="B2" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="Q2" s="8">
         <v>1</v>
@@ -1927,13 +1916,13 @@
     </row>
     <row r="3" spans="1:19">
       <c r="B3" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -1942,7 +1931,7 @@
         <v>-1</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="Q3" s="8">
         <v>1</v>
@@ -1953,25 +1942,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G4" s="3">
         <v>20</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="Q4" s="8">
         <v>2</v>
@@ -1982,25 +1971,25 @@
     </row>
     <row r="5" spans="1:19" ht="29">
       <c r="B5" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G5" s="3">
         <v>10</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="Q5" s="8">
         <v>3</v>
@@ -2014,22 +2003,22 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G6" s="3">
         <v>20</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>11</v>
@@ -2046,25 +2035,25 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C7" s="3">
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G7" s="3">
         <v>20</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q7" s="8">
         <v>1</v>
@@ -2078,22 +2067,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G8" s="3">
         <v>40</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="Q8" s="8">
         <v>1</v>
@@ -2104,22 +2093,22 @@
     </row>
     <row r="9" spans="1:19">
       <c r="B9" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G9" s="3">
         <v>30</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="Q9" s="8">
         <v>2</v>
@@ -2130,22 +2119,22 @@
     </row>
     <row r="10" spans="1:19">
       <c r="B10" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G10" s="3">
         <v>20</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="Q10" s="8">
         <v>3</v>
@@ -2156,22 +2145,22 @@
     </row>
     <row r="11" spans="1:19">
       <c r="B11" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="Q11" s="8">
         <v>4</v>
@@ -2182,19 +2171,19 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I12" s="3">
         <v>1</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="Q12" s="8">
         <v>1</v>
@@ -2202,19 +2191,19 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I13" s="3">
         <v>1</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="Q13" s="8">
         <v>2</v>
@@ -2222,19 +2211,19 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I14" s="3">
         <v>1</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="Q14" s="8">
         <v>3</v>
@@ -2242,22 +2231,22 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I15" s="3">
         <v>2</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="Q15" s="8">
         <v>1</v>
@@ -2265,19 +2254,19 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I16" s="3">
         <v>1</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="Q16" s="8">
         <v>1</v>
@@ -2285,19 +2274,19 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I17" s="3">
         <v>1</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="Q17" s="8">
         <v>2</v>
@@ -2305,16 +2294,16 @@
     </row>
     <row r="18" spans="1:17">
       <c r="C18" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I18" s="3">
         <v>1</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q18" s="8">
         <v>1</v>
@@ -2322,16 +2311,16 @@
     </row>
     <row r="19" spans="1:17">
       <c r="C19" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I19" s="3">
         <v>1</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q19" s="8">
         <v>2</v>
@@ -2352,8 +2341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2416,34 +2405,34 @@
   <sheetData>
     <row r="1" spans="1:60" s="8" customFormat="1">
       <c r="A1" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>5</v>
@@ -2452,156 +2441,156 @@
         <v>4</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="O1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="R1" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="W1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Z1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE1" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF1" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH1" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI1" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ1" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK1" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="AL1" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN1" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AQ1" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="AR1" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS1" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT1" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU1" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="AV1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW1" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="AX1" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="AY1" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="AZ1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA1" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="BC1" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="S1" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="W1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y1" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z1" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA1" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC1" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD1" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE1" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF1" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG1" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH1" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI1" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ1" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="AK1" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL1" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="AM1" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN1" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO1" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="AP1" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="AQ1" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="AR1" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="AS1" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="AT1" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="AU1" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="AV1" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW1" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="AX1" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="AY1" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="AZ1" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="BA1" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="BB1" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="BC1" s="26" t="s">
-        <v>113</v>
-      </c>
       <c r="BD1" s="26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="BE1" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="BF1" s="27" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BG1" s="28" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="BH1" s="28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:60">
       <c r="A2" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C2" s="30">
         <v>62</v>
@@ -2610,7 +2599,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G2" s="31">
         <v>73</v>
@@ -2622,16 +2611,16 @@
         <v>1</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="O2" s="33" t="s">
         <v>6</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="R2" s="34">
         <v>34</v>
@@ -2648,13 +2637,13 @@
     </row>
     <row r="3" spans="1:60">
       <c r="M3" s="33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N3" s="33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="P3" s="34" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R3" s="34">
         <v>55</v>
@@ -2674,16 +2663,16 @@
     </row>
     <row r="4" spans="1:60">
       <c r="M4" s="33" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N4" s="33" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O4" s="33" t="s">
         <v>6</v>
       </c>
       <c r="P4" s="34" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="R4" s="34">
         <v>36.587000000000003</v>
@@ -2700,7 +2689,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F5" s="31">
         <v>96</v>
@@ -2712,13 +2701,13 @@
         <v>2</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="P5" s="34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="Q5" s="34">
         <v>96</v>
@@ -2732,7 +2721,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F6" s="31">
         <v>96</v>
@@ -2744,13 +2733,13 @@
         <v>3</v>
       </c>
       <c r="M6" s="33" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="N6" s="33" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="P6" s="34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="Q6" s="34">
         <v>96</v>
@@ -2761,13 +2750,13 @@
     </row>
     <row r="7" spans="1:60">
       <c r="M7" s="33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N7" s="33" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="P7" s="34" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="Q7" s="34">
         <v>96</v>
@@ -2781,7 +2770,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C8" s="30">
         <v>62</v>
@@ -2790,7 +2779,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F8" s="31">
         <v>16</v>
@@ -2802,13 +2791,13 @@
         <v>1</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="N8" s="33" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="P8" s="34" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="Q8" s="34">
         <v>16</v>
@@ -2819,16 +2808,16 @@
     </row>
     <row r="9" spans="1:60">
       <c r="M9" s="33" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="N9" s="33" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="O9" s="33" t="s">
         <v>6</v>
       </c>
       <c r="P9" s="34" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="R9" s="34">
         <v>9</v>
@@ -2839,10 +2828,10 @@
     </row>
     <row r="10" spans="1:60">
       <c r="A10" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C10" s="30">
         <v>62</v>
@@ -2851,7 +2840,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F10" s="31">
         <v>16</v>
@@ -2863,13 +2852,13 @@
         <v>1</v>
       </c>
       <c r="M10" s="33" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="N10" s="33" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="P10" s="34" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="Q10" s="34">
         <v>16</v>
@@ -2880,16 +2869,16 @@
     </row>
     <row r="11" spans="1:60">
       <c r="M11" s="33" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="N11" s="33" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="O11" s="33" t="s">
         <v>6</v>
       </c>
       <c r="P11" s="34" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="R11" s="34">
         <v>10</v>
@@ -2900,10 +2889,10 @@
     </row>
     <row r="12" spans="1:60">
       <c r="A12" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C12" s="30">
         <v>55</v>
@@ -2912,7 +2901,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F12" s="31">
         <v>54</v>
@@ -2924,13 +2913,13 @@
         <v>1</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N12" s="33" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="P12" s="34" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="Q12" s="34">
         <v>54</v>
@@ -2947,19 +2936,19 @@
     </row>
     <row r="13" spans="1:60">
       <c r="E13" s="31" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="M13" s="33" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="N13" s="33" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="O13" s="33" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="P13" s="34" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="Q13" s="34">
         <v>9</v>
@@ -2968,7 +2957,7 @@
         <v>1</v>
       </c>
       <c r="Y13" s="36" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="Z13" s="36">
         <v>9</v>
@@ -2977,7 +2966,7 @@
         <v>1</v>
       </c>
       <c r="AE13" s="38" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="AF13" s="38">
         <v>9</v>
@@ -2992,7 +2981,7 @@
         <v>1</v>
       </c>
       <c r="AQ13" s="42" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AR13" s="42">
         <v>9</v>
@@ -3001,7 +2990,7 @@
         <v>1</v>
       </c>
       <c r="AW13" s="30" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="AX13" s="30">
         <v>9</v>
@@ -3015,7 +3004,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F14" s="31">
         <v>54</v>
@@ -3027,13 +3016,13 @@
         <v>1</v>
       </c>
       <c r="M14" s="33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N14" s="33" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="P14" s="34" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="Q14" s="34">
         <v>54</v>
@@ -3050,19 +3039,19 @@
     </row>
     <row r="15" spans="1:60">
       <c r="E15" s="31" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="M15" s="33" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="N15" s="33" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="O15" s="33" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="P15" s="34" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="Q15" s="34">
         <v>9</v>
@@ -3071,7 +3060,7 @@
         <v>1</v>
       </c>
       <c r="Y15" s="36" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="Z15" s="36">
         <v>9</v>
@@ -3080,7 +3069,7 @@
         <v>1</v>
       </c>
       <c r="AE15" s="47" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="AF15" s="38">
         <v>9</v>
@@ -3095,7 +3084,7 @@
         <v>1</v>
       </c>
       <c r="AQ15" s="42" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="AR15" s="42">
         <v>9</v>
@@ -3104,7 +3093,7 @@
         <v>1</v>
       </c>
       <c r="AW15" s="30" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="AX15" s="30">
         <v>9</v>
@@ -3118,7 +3107,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F16" s="31">
         <v>54</v>
@@ -3130,13 +3119,13 @@
         <v>1</v>
       </c>
       <c r="M16" s="33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N16" s="33" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="P16" s="34" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="Q16" s="34">
         <v>54</v>
@@ -3153,19 +3142,19 @@
     </row>
     <row r="17" spans="1:51">
       <c r="E17" s="48" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="M17" s="33" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="N17" s="33" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="O17" s="33" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="P17" s="34" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="Q17" s="34">
         <v>9</v>
@@ -3174,7 +3163,7 @@
         <v>1</v>
       </c>
       <c r="Y17" s="36" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="Z17" s="36">
         <v>9</v>
@@ -3183,7 +3172,7 @@
         <v>1</v>
       </c>
       <c r="AE17" s="47" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="AF17" s="38">
         <v>9</v>
@@ -3198,7 +3187,7 @@
         <v>1</v>
       </c>
       <c r="AQ17" s="42" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="AR17" s="42">
         <v>9</v>
@@ -3207,7 +3196,7 @@
         <v>1</v>
       </c>
       <c r="AW17" s="30" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AX17" s="30">
         <v>9</v>
@@ -3221,7 +3210,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F18" s="31">
         <v>54</v>
@@ -3233,13 +3222,13 @@
         <v>1</v>
       </c>
       <c r="M18" s="33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N18" s="33" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="P18" s="34" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="Q18" s="34">
         <v>54</v>
@@ -3257,16 +3246,16 @@
     </row>
     <row r="19" spans="1:51">
       <c r="E19" s="48" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="M19" s="33" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="N19" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="P19" s="34" t="s">
         <v>133</v>
-      </c>
-      <c r="P19" s="34" t="s">
-        <v>138</v>
       </c>
       <c r="Q19" s="34">
         <v>54</v>
@@ -3278,10 +3267,10 @@
     </row>
     <row r="20" spans="1:51">
       <c r="A20" s="10" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C20" s="30">
         <v>55</v>
@@ -3290,7 +3279,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F20" s="31">
         <v>3</v>
@@ -3302,10 +3291,10 @@
         <v>1</v>
       </c>
       <c r="M20" s="33" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="P20" s="34" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="Q20" s="34">
         <v>3</v>
@@ -3325,10 +3314,10 @@
         <v>2</v>
       </c>
       <c r="M21" s="33" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="P21" s="34" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="Q21" s="34">
         <v>9</v>
@@ -3336,7 +3325,7 @@
     </row>
     <row r="22" spans="1:51">
       <c r="A22" s="10" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C22" s="30">
         <v>60</v>
@@ -3352,20 +3341,6 @@
       </c>
       <c r="L22" s="32">
         <v>1</v>
-      </c>
-      <c r="M22" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="O22" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:51">
-      <c r="M23" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="O23" s="33" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:51">
@@ -3406,19 +3381,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3440,7 +3415,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -3451,10 +3426,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -3465,7 +3440,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3481,138 +3456,55 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1">
+    <row r="1" spans="1:2" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="G2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2">
         <v>0.5</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="G3">
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
         <v>0.5</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>0.5</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>0.5</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="G6">
-        <v>0.5</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>